<commit_message>
2022.01.09 | Hu Wenqiang | Repaired the Bug of Not Drawing the Webpage
</commit_message>
<xml_diff>
--- a/T3/2020.12.1.xlsx
+++ b/T3/2020.12.1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -66,18 +66,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -446,13 +446,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="31"/>
-    <col customWidth="1" max="2" min="2" width="19"/>
-    <col customWidth="1" max="3" min="3" width="8"/>
-    <col customWidth="1" max="4" min="4" width="15"/>
-    <col customWidth="1" max="5" min="5" width="20"/>
-    <col customWidth="1" max="6" min="6" width="20"/>
-    <col customWidth="1" max="7" min="7" width="80"/>
+    <col width="31" customWidth="1" min="1" max="1"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="80" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -495,1825 +495,1824 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020-12-01 22:21:17</t>
+          <t>2020-12-01 05:43:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>422825198810114454</t>
+          <t>440200198007168914</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>张荣</t>
+          <t>冯宇</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>18248480965</t>
+          <t>15157132991</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>119.944296584982</v>
+        <v>119.934881684961</v>
       </c>
       <c r="F2" t="n">
-        <v>30.097262635875</v>
+        <v>30.063084431323</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区银湖街道高富路富通高桥工场</t>
+          <t>浙江省杭州市富阳区富春街道文采路202号金色家园(金桥北路)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2020-12-01 21:21:10</t>
+          <t>2020-12-01 05:58:00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>211381199612278296</t>
+          <t>610524199407192917</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>林红霞</t>
+          <t>蔡秀云</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>13500599252</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>119.945421709799</v>
-      </c>
-      <c r="F3" t="n">
-        <v>30.045358805853</v>
+          <t>18281858028</t>
+        </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道菜市街70号</t>
+          <t>error: 输入坐标不全!</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2020-12-01 21:20:13</t>
+          <t>2020-12-01 06:29:55</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>320831199506081068</t>
+          <t>130110201406057962</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>吴帅</t>
+          <t>王娟</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15057188534</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>119.934256663262</v>
-      </c>
-      <c r="F4" t="n">
-        <v>30.038822422433</v>
+          <t>13738014816</t>
+        </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道南渠绿道</t>
+          <t>error: 输入坐标不全!</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2020-12-01 21:13:39</t>
+          <t>2020-12-01 06:33:26</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>230805198304179586</t>
+          <t>331024199501036087</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>李桂兰</t>
+          <t>阎春梅</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>15085699499</t>
+          <t>15156483403</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>119.75001</v>
+        <v>119.885075462635</v>
       </c>
       <c r="F5" t="n">
-        <v>29.99805</v>
+        <v>29.897829252702</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇5号路</t>
+          <t>浙江省杭州市富阳区常安镇双隆控股集团</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2020-12-01 20:46:16</t>
+          <t>2020-12-01 07:11:06</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>361127200007015606</t>
+          <t>410425198608116258</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>王丽</t>
+          <t>胡超</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>15938399252</t>
+          <t>13606609521</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>119.946664272439</v>
+        <v>119.628240003265</v>
       </c>
       <c r="F6" t="n">
-        <v>30.046655271192</v>
+        <v>29.961270004524</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道回春路回春路-道路停车位</t>
+          <t>浙江省杭州市富阳区胥口镇水坞水库</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2020-12-01 20:12:34</t>
+          <t>2020-12-01 07:12:02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>410800198209196611</t>
+          <t>469029200310029400</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>张辉</t>
+          <t>程杰</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>18357147883</t>
+          <t>13806516227</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>119.971528287016</v>
+        <v>119.730270000247</v>
       </c>
       <c r="F7" t="n">
-        <v>30.038272696524</v>
+        <v>29.936659999961</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区春江街道大桥南路</t>
+          <t>浙江省杭州市富阳区渌渚镇碧沼寺</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2020-12-01 19:58:38</t>
+          <t>2020-12-01 07:18:18</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>310151201609227483</t>
+          <t>511903201305174205</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>黄彬</t>
+          <t>张玉珍</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>18768118774</t>
+          <t>15068120595</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>119.870459933587</v>
+        <v>119.920252972396</v>
       </c>
       <c r="F8" t="n">
-        <v>29.914567752373</v>
+        <v>30.050301859895</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区场口镇瓜桥江绿道</t>
+          <t>浙江省杭州市富阳区富春街道浪漫香槟(东区)浪漫香槟东区</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2020-12-01 19:27:51</t>
+          <t>2020-12-01 07:22:28</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>140727199902258044</t>
+          <t>330402200511053516</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>裘亮</t>
+          <t>李玉</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>15258868990</t>
+          <t>15267012370</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>119.95238</v>
+        <v>119.934402483888</v>
       </c>
       <c r="F9" t="n">
-        <v>30.07537</v>
+        <v>30.090534554371</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道庭庐餐厅融创富春壹号院</t>
+          <t>浙江省杭州市富阳区银湖街道万达同心湾(建设中)杭州富阳万达广场</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2020-12-01 19:21:19</t>
+          <t>2020-12-01 07:40:36</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>130626199411096219</t>
+          <t>420000196511075182</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>蒲柳</t>
+          <t>方玉华</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>15324476439</t>
+          <t>13858048604</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>119.72229</v>
+        <v>120.09642</v>
       </c>
       <c r="F10" t="n">
-        <v>29.9667</v>
+        <v>30.04937</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇430县道</t>
+          <t>浙江省杭州市富阳区渔山乡渔葛线</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2020-12-01 19:20:55</t>
+          <t>2020-12-01 07:49:19</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>421223199805018239</t>
+          <t>51118119951001381X</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>吴勇</t>
+          <t>吴鹏</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>18958171357</t>
-        </is>
+          <t>15869103863</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>119.839629365219</v>
+      </c>
+      <c r="F11" t="n">
+        <v>29.985965842432</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>error: 输入坐标不全!</t>
+          <t>浙江省杭州市富阳区鹿山街道华家</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2020-12-01 19:16:35</t>
+          <t>2020-12-01 07:55:28</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>511526199609013761</t>
+          <t>450324199806012791</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>高倩</t>
+          <t>余静</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>15988180938</t>
+          <t>18858121141</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>119.917848478986</v>
+        <v>119.884279760809</v>
       </c>
       <c r="F12" t="n">
-        <v>30.066553789586</v>
+        <v>30.117161307504</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道孙油线</t>
+          <t>浙江省杭州市富阳区银湖街道423县道</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2020-12-01 19:03:05</t>
+          <t>2020-12-01 07:56:16</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>130302198306122348</t>
+          <t>130481199512241239</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>江龙</t>
+          <t>赵琳</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13706816295</t>
+          <t>13967103871</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>119.988101918469</v>
+        <v>119.936719993773</v>
       </c>
       <c r="F13" t="n">
-        <v>30.069178386718</v>
+        <v>30.043488856435</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区东洲街道高尔夫路537号富阳东洲民丰小学</t>
+          <t>浙江省杭州市富阳区富春街道城市花园(秦望路)龙祥城市花园</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2020-12-01 18:36:23</t>
+          <t>2020-12-01 08:00:31</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>45092419970517118X</t>
+          <t>421222199809034969</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>张阳</t>
+          <t>陈琴</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13777359971</t>
+          <t>13858071281</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>119.961144852051</v>
+        <v>119.906691219552</v>
       </c>
       <c r="F14" t="n">
-        <v>30.030052570865</v>
+        <v>30.048983698148</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区春江街道江南中学</t>
+          <t>浙江省杭州市富阳区富春街道华虹路</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2020-12-01 18:31:49</t>
+          <t>2020-12-01 08:04:35</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>360900200004277902</t>
+          <t>140403201804261912</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>赵旭</t>
+          <t>郑莹</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>15967192402</t>
+          <t>13362144407</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>119.938346115923</v>
+        <v>119.920835130529</v>
       </c>
       <c r="F15" t="n">
-        <v>30.05770211121</v>
+        <v>30.013759836072</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道文教北路永兴学校教师公寓</t>
+          <t>浙江省杭州市富阳区鹿山街道福济庙</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2020-12-01 18:31:49</t>
+          <t>2020-12-01 08:04:40</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>220881199511247851</t>
+          <t>211282199509102728</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>张凤英</t>
+          <t>敖英</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>15669536808</t>
+          <t>13777491569</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>119.971807169923</v>
+        <v>119.873099285498</v>
       </c>
       <c r="F16" t="n">
-        <v>30.031203474998</v>
+        <v>29.988102645403</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区春江街道上海外国语大学附属杭州学校(建设中)</t>
+          <t>浙江省杭州市富阳区鹿山街道杭州安澜海业动力机械有限公司</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2020-12-01 18:31:26</t>
+          <t>2020-12-01 08:07:16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>511324199305085738</t>
+          <t>321300199611276069</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>杨利</t>
+          <t>周玉梅</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>13777853631</t>
+          <t>18758002725</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>119.87356</v>
+        <v>119.935197936995</v>
       </c>
       <c r="F17" t="n">
-        <v>29.99376</v>
+        <v>30.053488762548</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区鹿山街道永盛科技有限公司(流体事业部)</t>
+          <t>浙江省杭州市富阳区富春街道永兴花园凤凰苑(凤浦路)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2020-12-01 18:31:10</t>
+          <t>2020-12-01 08:08:42</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>21072619701115157X</t>
+          <t>440800196508026141</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>王兵</t>
+          <t>黄霞</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>15158830484</t>
+          <t>13357111728</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>119.954771379323</v>
+        <v>119.946324623285</v>
       </c>
       <c r="F18" t="n">
-        <v>30.057509470828</v>
+        <v>30.066249466767</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道光明路9-1号</t>
+          <t>浙江省杭州市富阳区富春街道公望街虎山雅苑</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2020-12-01 18:29:40</t>
+          <t>2020-12-01 08:12:47</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>430602199608232632</t>
+          <t>230605198211158179</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>裴璐</t>
+          <t>李平</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13362568609</t>
+          <t>13588372438</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>119.893050007208</v>
+        <v>119.985952799662</v>
       </c>
       <c r="F19" t="n">
-        <v>30.064440002077</v>
+        <v>30.067752766367</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道杭州潮汛流体控制科技有限公司</t>
+          <t>浙江省杭州市富阳区东洲街道浙江富春江光电科技有限公司富春江集团光通信工业园</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2020-12-01 18:29:16</t>
+          <t>2020-12-01 08:18:00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>620502200404014890</t>
+          <t>530125198308111288</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>张彬</t>
+          <t>杨丽</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>15888809563</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>119.697746222762</v>
+        <v>119.974322358456</v>
       </c>
       <c r="F20" t="n">
-        <v>29.984817036958</v>
+        <v>30.162255520543</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区胥口镇05省道</t>
+          <t>浙江省杭州市富阳区银湖街道九龙仓·雍景山九龙仓·雍景山城</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2020-12-01 18:22:06</t>
+          <t>2020-12-01 08:18:05</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>130530199303287789</t>
+          <t>659006201203234308</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>纪欣</t>
+          <t>赵云</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>15972406141</t>
+          <t>18658042800</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>119.988072555233</v>
+        <v>119.959673357473</v>
       </c>
       <c r="F21" t="n">
-        <v>30.069137945355</v>
+        <v>30.053757333239</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区东洲街道高尔夫路537号富阳东洲民丰小学</t>
+          <t>浙江省杭州市富阳区富春街道达夫路145号</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2020-12-01 18:18:00</t>
+          <t>2020-12-01 08:20:56</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>320612200909197407</t>
+          <t>610304200312125147</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>王杰</t>
+          <t>卢玉兰</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>18314899806</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>120.030650057354</v>
-      </c>
-      <c r="F22" t="n">
-        <v>30.033001385081</v>
+          <t>13803990917</t>
+        </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区灵桥镇浙江金东纸业</t>
+          <t>error: 输入坐标不全!</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2020-12-01 18:15:39</t>
+          <t>2020-12-01 08:24:36</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>420702198710241956</t>
+          <t>310104199001029361</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>陈秀荣</t>
+          <t>周佳</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>18327553759</t>
+          <t>18758087628</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>119.891836841929</v>
+        <v>119.748167457896</v>
       </c>
       <c r="F23" t="n">
-        <v>30.05821063413</v>
+        <v>30.001813667236</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道双峰山</t>
+          <t>浙江省杭州市富阳区新登镇贝山路</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2020-12-01 18:08:38</t>
+          <t>2020-12-01 08:24:41</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>140703201909156648</t>
+          <t>370613199408051995</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>江桂荣</t>
+          <t>郭勇</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13675876638</t>
+          <t>13588818578</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>119.962443727165</v>
+        <v>119.95848734533</v>
       </c>
       <c r="F24" t="n">
-        <v>30.05409731211</v>
+        <v>30.055637341849</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道大桥路159号富阳区城市森林公园</t>
+          <t>浙江省杭州市富阳区富春街道大桥路63号明裕花苑(大桥路)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2020-12-01 18:06:50</t>
+          <t>2020-12-01 08:42:08</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>410721198907254459</t>
+          <t>331121200011172184</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>胡琴</t>
+          <t>范淑英</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13588396058</t>
+          <t>15858189066</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>119.744834</v>
+        <v>119.940073401748</v>
       </c>
       <c r="F25" t="n">
-        <v>30.005376</v>
+        <v>30.049084693107</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇沃新线</t>
+          <t>浙江省杭州市富阳区富春街道金都铭苑(秋月路)金都铭苑东区</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2020-12-01 17:50:33</t>
+          <t>2020-12-01 08:53:05</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>130582199505259141</t>
+          <t>450108200402126076</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>孙瑞</t>
+          <t>王鹏</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13336027313</t>
+          <t>13567138273</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>119.93635505368</v>
+        <v>119.946904588043</v>
       </c>
       <c r="F26" t="n">
-        <v>30.053672876579</v>
+        <v>30.068024227572</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道凤浦社区飞虹·丁香花园(金桥北路)</t>
+          <t>浙江省杭州市富阳区富春街道天时苑(西区)金门东望大厦</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2020-12-01 17:40:18</t>
+          <t>2020-12-01 08:54:56</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>431302199901045021</t>
+          <t>440114200005255494</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>罗岩</t>
+          <t>冉晨</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>15957128398</t>
+          <t>15658115330</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>119.910291130682</v>
+        <v>119.925901060393</v>
       </c>
       <c r="F27" t="n">
-        <v>30.063990017737</v>
+        <v>30.070107726686</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道公望街1165号汉邦钢材市场北区</t>
+          <t>浙江省杭州市富阳区富春街道金苑路</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2020-12-01 17:38:40</t>
+          <t>2020-12-01 09:04:14</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>520281201703269746</t>
+          <t>430423198406157378</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>孙建平</t>
+          <t>汪秀梅</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>13968164976</t>
+          <t>13221099822</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>119.937601140995</v>
+        <v>119.87082</v>
       </c>
       <c r="F28" t="n">
-        <v>30.030894926297</v>
+        <v>29.97833</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道富春第七小学</t>
+          <t>浙江省杭州市富阳区鹿山街道S43杭州绕城西复线</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2020-12-01 17:29:05</t>
+          <t>2020-12-01 09:08:36</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>371425199411046877</t>
+          <t>632723198403048091</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>胡婷</t>
+          <t>吴岩</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>17706442283</t>
+          <t>15824190404</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>119.92575</v>
+        <v>119.736699662198</v>
       </c>
       <c r="F29" t="n">
-        <v>30.02332</v>
+        <v>29.96761302358</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区鹿山街道驯雉小学</t>
+          <t>浙江省杭州市富阳区新登镇登城北路19号</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2020-12-01 17:21:56</t>
+          <t>2020-12-01 10:20:09</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>130321198603056999</t>
+          <t>230183199606275181</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>杨志强</t>
+          <t>李淑兰</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>13968019333</t>
-        </is>
+          <t>13584838199</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>119.971528287016</v>
+      </c>
+      <c r="F30" t="n">
+        <v>30.038272696524</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>error: 输入坐标不全!</t>
+          <t>浙江省杭州市富阳区春江街道大桥南路</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2020-12-01 17:21:38</t>
+          <t>2020-12-01 10:20:20</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>320118201302072910</t>
+          <t>610803201510213143</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>曾旭</t>
+          <t>张坤</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>13626713248</t>
+          <t>13968071566</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>119.914827000385</v>
+        <v>119.940044577139</v>
       </c>
       <c r="F31" t="n">
-        <v>30.054731999654</v>
+        <v>30.053073402269</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道秦忆荣府北区</t>
+          <t>浙江省杭州市富阳区富春街道凤浦路</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2020-12-01 17:17:21</t>
+          <t>2020-12-01 10:23:40</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>140404201803243997</t>
+          <t>230123199105253957</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>刘雪</t>
+          <t>王萍</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>13911869797</t>
+          <t>15568233366</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>119.912227902269</v>
+        <v>119.941568251921</v>
       </c>
       <c r="F32" t="n">
-        <v>30.009356612782</v>
+        <v>30.072021320619</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区鹿山街道富冶</t>
+          <t>浙江省杭州市富阳区富春街道富春印象金座富春新天地</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2020-12-01 17:14:27</t>
+          <t>2020-12-01 10:26:05</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>21110420160301771X</t>
+          <t>350800199602085481</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>朱平</t>
+          <t>刘淑兰</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>18058819611</t>
+          <t>13868127754</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>119.609769267959</v>
+        <v>119.872802703836</v>
       </c>
       <c r="F33" t="n">
-        <v>30.034007878132</v>
+        <v>29.988073551047</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区洞桥镇胥高线</t>
+          <t>浙江省杭州市富阳区鹿山街道杭州安澜海业动力机械有限公司</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2020-12-01 17:12:40</t>
+          <t>2020-12-01 10:26:43</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>520325199808286280</t>
+          <t>653123198508197589</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>张宁</t>
+          <t>王芳</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>15088651898</t>
+          <t>15888825716</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>119.66851</v>
+        <v>119.950580984148</v>
       </c>
       <c r="F34" t="n">
-        <v>29.98639</v>
+        <v>30.052734196765</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区胥口镇泥塍头</t>
+          <t>浙江省杭州市富阳区富春街道新兴路122号百合景苑</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2020-12-01 17:12:08</t>
+          <t>2020-12-01 10:31:53</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>371721200011076141</t>
+          <t>341102199204084962</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>齐宁</t>
+          <t>李秀芳</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>13588390997</t>
+          <t>13706505205</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>119.866428407807</v>
+        <v>119.88067</v>
       </c>
       <c r="F35" t="n">
-        <v>30.039808618221</v>
+        <v>30.12405</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道唯益生态农场</t>
+          <t>浙江省杭州市富阳区银湖街道杭州市富阳区银湖街道新义小学</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2020-12-01 17:07:01</t>
+          <t>2020-12-01 10:35:20</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>441802199205254646</t>
+          <t>411500199808167299</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>杨兵</t>
+          <t>陈帅</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15967114462</t>
+          <t>18067904810</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>119.978243327095</v>
+        <v>119.92601</v>
       </c>
       <c r="F36" t="n">
-        <v>30.077620959272</v>
+        <v>29.9352</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区东洲街道佑昌意菲司图(杭州)金属制品有限公司</t>
+          <t>浙江省杭州市富阳区环山乡G25长深高速</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2020-12-01 17:03:16</t>
+          <t>2020-12-01 10:39:08</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>331022199412259702</t>
+          <t>150825200311221952</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>邵晨</t>
+          <t>龚凯</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>18324490018</t>
+          <t>15088698899</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>119.93654794656</v>
+        <v>119.878397077327</v>
       </c>
       <c r="F37" t="n">
-        <v>30.054769047965</v>
+        <v>30.042040616969</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道飞虹·丁香花园(金桥北路)</t>
+          <t>浙江省杭州市富阳区富春街道320国道辅路</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2020-12-01 16:58:25</t>
+          <t>2020-12-01 10:44:48</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>120102198805063327</t>
+          <t>532601201001289404</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>李强</t>
+          <t>叶玉英</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15382328993</t>
+          <t>13588760817</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>119.8514063421</v>
+        <v>119.752260956386</v>
       </c>
       <c r="F38" t="n">
-        <v>29.988830761241</v>
+        <v>30.003557215076</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区鹿山街道大树下</t>
+          <t>浙江省杭州市富阳区新登镇军堰路生威新能源</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2020-12-01 16:45:08</t>
+          <t>2020-12-01 10:46:02</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>623025199904234990</t>
+          <t>320282199603151918</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>王宁</t>
+          <t>钟辉</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15988879169</t>
+          <t>18258212106</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>119.746293071808</v>
+        <v>120.003246763257</v>
       </c>
       <c r="F39" t="n">
-        <v>30.000392682626</v>
+        <v>30.052777473716</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇302省道</t>
+          <t>浙江省杭州市富阳区东洲街道何埭机埠</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2020-12-01 16:31:54</t>
+          <t>2020-12-01 10:49:36</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>530722200207202520</t>
+          <t>632622196512049711</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>魏强</t>
+          <t>张红</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13819164910</t>
+          <t>15067175728</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>119.920751734744</v>
+        <v>119.908879053854</v>
       </c>
       <c r="F40" t="n">
-        <v>30.063992918354</v>
+        <v>30.068399940499</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道西环北路225号</t>
+          <t>浙江省杭州市富阳区富春街道阳陂湖小火车南站阳陂湖P1停车场</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2020-12-01 16:31:49</t>
+          <t>2020-12-01 11:08:06</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>141029200007046791</t>
+          <t>350629198511195738</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>吴金凤</t>
+          <t>张伟</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13968174817</t>
+          <t>13675875155</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>120.028376222184</v>
+        <v>119.94824</v>
       </c>
       <c r="F41" t="n">
-        <v>30.064818696745</v>
+        <v>30.06749</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区东洲街道湖上沙村</t>
+          <t>浙江省杭州市富阳区富春街道天时苑(西区)天时苑西区</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2020-12-01 16:29:09</t>
+          <t>2020-12-01 11:20:14</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>522627198302188970</t>
+          <t>370285199711144158</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>杨云</t>
+          <t>李丹</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>18329188508</t>
+          <t>13456836266</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>119.93543129835</v>
+        <v>119.975811008628</v>
       </c>
       <c r="F42" t="n">
-        <v>30.058400180538</v>
+        <v>30.02174502131</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道德邻公寓富阳区永兴学校</t>
+          <t>浙江省杭州市富阳区春江街道春江街道直塘村文化活动中心</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2020-12-01 16:27:43</t>
+          <t>2020-12-01 11:23:24</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>530481201904041070</t>
+          <t>361103201504145712</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>温强</t>
+          <t>向玉华</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>15867171758</t>
+          <t>13868163877</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>119.736853485196</v>
+        <v>119.94824</v>
       </c>
       <c r="F43" t="n">
-        <v>29.98939705182</v>
+        <v>30.06749</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇四号路</t>
+          <t>浙江省杭州市富阳区富春街道天时苑(西区)天时苑西区</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2020-12-01 16:24:38</t>
+          <t>2020-12-01 11:32:02</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>610302199809281040</t>
+          <t>360827200012163053</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>赵丽丽</t>
+          <t>姜帆</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>15824171348</t>
+          <t>13705711539</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>119.733700301888</v>
+        <v>119.937732806213</v>
       </c>
       <c r="F44" t="n">
-        <v>29.964790850403</v>
+        <v>30.052326877704</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇裕达饼家(新兴路店)</t>
+          <t>浙江省杭州市富阳区富春街道凤凰小区</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2020-12-01 16:22:17</t>
+          <t>2020-12-01 11:35:34</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>513226199904235573</t>
+          <t>610627199601262610</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>李欣</t>
+          <t>刘桂花</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>13221828587</t>
+          <t>13429178089</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>119.936079476613</v>
+        <v>119.960879653585</v>
       </c>
       <c r="F45" t="n">
-        <v>30.062299368257</v>
+        <v>30.130014881814</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道郦城</t>
+          <t>浙江省杭州市富阳区银湖街道上上线</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2020-12-01 16:10:20</t>
+          <t>2020-12-01 11:38:10</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>433124199012225830</t>
+          <t>441223198805172374</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>刘伟</t>
+          <t>余波</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13605574551</t>
+          <t>13968052087</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>119.939331287876</v>
+        <v>119.950429002502</v>
       </c>
       <c r="F46" t="n">
-        <v>30.037166138909</v>
+        <v>30.051439174845</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道文教路杭州富阳水务管道安装有限公司</t>
+          <t>浙江省杭州市富阳区富春街道渔种场路64号</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2020-12-01 15:48:22</t>
+          <t>2020-12-01 11:40:32</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>150122196009192963</t>
+          <t>640105200211029288</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>李建军</t>
+          <t>张莹</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>15858160116</t>
+          <t>15158845772</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>119.946324623285</v>
+        <v>119.966768963353</v>
       </c>
       <c r="F47" t="n">
-        <v>30.066249466767</v>
+        <v>30.133722600522</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道公望街虎山雅苑</t>
+          <t>浙江省杭州市富阳区银湖街道龙溪北路</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2020-12-01 15:40:12</t>
+          <t>2020-12-01 11:52:26</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>440303199007136727</t>
+          <t>451402200207223734</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>刘洋</t>
+          <t>张斌</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13588282970</t>
+          <t>13732236310</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>119.715405693318</v>
+        <v>119.93773524959</v>
       </c>
       <c r="F48" t="n">
-        <v>29.878966732299</v>
+        <v>30.05909982042</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区渌渚镇大俞线</t>
+          <t>浙江省杭州市富阳区富春街道文居街德邻公寓</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2020-12-01 15:36:09</t>
+          <t>2020-12-01 11:55:45</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>360826200002072688</t>
+          <t>140000197111029467</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>严秀云</t>
+          <t>萧海燕</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13588397358</t>
+          <t>15925626674</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>119.792536773035</v>
+        <v>119.50874421565</v>
       </c>
       <c r="F49" t="n">
-        <v>29.884492806711</v>
+        <v>30.065402515467</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新桐乡桐洲绿道桐洲岛</t>
+          <t>浙江省杭州市桐庐县分水镇兑百线</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2020-12-01 15:25:31</t>
+          <t>2020-12-01 12:08:36</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>620724200208057999</t>
+          <t>630223201309169386</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>鲁帅</t>
+          <t>林欣</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>18658808055</t>
+          <t>15397123912</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>119.94854864858</v>
+        <v>119.94152</v>
       </c>
       <c r="F50" t="n">
-        <v>30.058028610008</v>
+        <v>30.06786</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道孙权路28-2号现代技术培训学校</t>
+          <t>浙江省杭州市富阳区富春街道新汇社区居务监督委员会赵家埠弄-道路停车位</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2020-12-01 15:16:18</t>
+          <t>2020-12-01 12:17:36</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>42092319931018251X</t>
+          <t>130923199605033053</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>毕彬</t>
+          <t>王秀英</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13645815561</t>
+          <t>18768187282</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>119.960484596484</v>
+        <v>119.77364</v>
       </c>
       <c r="F51" t="n">
-        <v>30.051685506887</v>
+        <v>30.00227</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道龙浦街128号富阳龙浦大酒店</t>
+          <t>浙江省杭州市富阳区新登镇宝万线</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2020-12-01 15:09:12</t>
+          <t>2020-12-01 12:38:03</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>231224199901079112</t>
+          <t>65312719521212477X</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>刘辉</t>
+          <t>黎强</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13588380680</t>
+          <t>15824171507</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>119.910831936552</v>
+        <v>119.932706608028</v>
       </c>
       <c r="F52" t="n">
-        <v>30.087445577424</v>
+        <v>30.050724801629</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区银湖街道周长线</t>
+          <t>浙江省杭州市富阳区富春街道金平路15号东方茂购物中心</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2020-12-01 15:03:55</t>
+          <t>2020-12-01 12:41:18</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>130407201601229756</t>
+          <t>620921200204197208</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>黄秀华</t>
+          <t>傅秀芳</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>18868757608</t>
+          <t>13989836682</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>119.937613994071</v>
+        <v>119.923208512268</v>
       </c>
       <c r="F53" t="n">
-        <v>30.037526829461</v>
+        <v>30.046899745452</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道现代肖邦(文教路)现代肖邦东区</t>
+          <t>浙江省杭州市富阳区富春街道横凉亭路辅路</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2020-12-01 15:03:10</t>
+          <t>2020-12-01 12:46:46</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>441322198811176493</t>
+          <t>460105200204252904</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>陈瑞</t>
+          <t>房明</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>18868723394</t>
+          <t>13819137543</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>119.735965</v>
+        <v>119.98592</v>
       </c>
       <c r="F54" t="n">
-        <v>29.967663</v>
+        <v>30.06812</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇登城北路13号</t>
+          <t>浙江省杭州市富阳区东洲街道浙江富春江光电科技有限公司富春江集团光通信工业园</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2020-12-01 14:59:37</t>
+          <t>2020-12-01 12:49:43</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>150428198308097660</t>
+          <t>620103196208076141</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>刘霞</t>
+          <t>林秀芳</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13173645515</t>
-        </is>
+          <t>15967166330</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>119.903789189148</v>
+      </c>
+      <c r="F55" t="n">
+        <v>30.096522847424</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>error: 输入坐标不全!</t>
+          <t>浙江省杭州市富阳区银湖街道周长线</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2020-12-01 14:41:24</t>
+          <t>2020-12-01 12:54:41</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>610700199609228076</t>
+          <t>370105197405128313</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>郑亮</t>
+          <t>严东</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>15957160099</t>
+          <t>18258238385</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>119.978561027168</v>
+        <v>119.945374918468</v>
       </c>
       <c r="F56" t="n">
-        <v>30.075920031334</v>
+        <v>30.06074222873</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区东洲街道大岭山路中恒电气</t>
+          <t>浙江省杭州市富阳区富春街道兴达路朗庭宾馆(文居街)</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2020-12-01 14:02:41</t>
+          <t>2020-12-01 13:10:13</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>340811200504078870</t>
+          <t>41042319830808540X</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>赵宁</t>
+          <t>刘飞</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13968144854</t>
-        </is>
-      </c>
-      <c r="E57" t="n">
-        <v>119.93892</v>
-      </c>
-      <c r="F57" t="n">
-        <v>30.0598</v>
+          <t>18758200922</t>
+        </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道阳光里</t>
+          <t>error: 输入坐标不全!</t>
         </is>
       </c>
     </row>
@@ -2353,1828 +2352,1829 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2020-12-01 13:10:13</t>
+          <t>2020-12-01 14:02:41</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>41042319830808540X</t>
+          <t>340811200504078870</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>刘飞</t>
+          <t>赵宁</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>18758200922</t>
-        </is>
+          <t>13968144854</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>119.93892</v>
+      </c>
+      <c r="F59" t="n">
+        <v>30.0598</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>error: 输入坐标不全!</t>
+          <t>浙江省杭州市富阳区富春街道阳光里</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2020-12-01 12:54:41</t>
+          <t>2020-12-01 14:41:24</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>370105197405128313</t>
+          <t>610700199609228076</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>严东</t>
+          <t>郑亮</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>18258238385</t>
+          <t>15957160099</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>119.945374918468</v>
+        <v>119.978561027168</v>
       </c>
       <c r="F60" t="n">
-        <v>30.06074222873</v>
+        <v>30.075920031334</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道兴达路朗庭宾馆(文居街)</t>
+          <t>浙江省杭州市富阳区东洲街道大岭山路中恒电气</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2020-12-01 12:49:43</t>
+          <t>2020-12-01 14:59:37</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>620103196208076141</t>
+          <t>150428198308097660</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>林秀芳</t>
+          <t>刘霞</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>15967166330</t>
-        </is>
-      </c>
-      <c r="E61" t="n">
-        <v>119.903789189148</v>
-      </c>
-      <c r="F61" t="n">
-        <v>30.096522847424</v>
+          <t>13173645515</t>
+        </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区银湖街道周长线</t>
+          <t>error: 输入坐标不全!</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2020-12-01 12:46:46</t>
+          <t>2020-12-01 15:03:10</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>460105200204252904</t>
+          <t>441322198811176493</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>房明</t>
+          <t>陈瑞</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13819137543</t>
+          <t>18868723394</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>119.98592</v>
+        <v>119.735965</v>
       </c>
       <c r="F62" t="n">
-        <v>30.06812</v>
+        <v>29.967663</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区东洲街道浙江富春江光电科技有限公司富春江集团光通信工业园</t>
+          <t>浙江省杭州市富阳区新登镇登城北路13号</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2020-12-01 12:41:18</t>
+          <t>2020-12-01 15:03:55</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>620921200204197208</t>
+          <t>130407201601229756</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>傅秀芳</t>
+          <t>黄秀华</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13989836682</t>
+          <t>18868757608</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>119.923208512268</v>
+        <v>119.937613994071</v>
       </c>
       <c r="F63" t="n">
-        <v>30.046899745452</v>
+        <v>30.037526829461</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道横凉亭路辅路</t>
+          <t>浙江省杭州市富阳区富春街道现代肖邦(文教路)现代肖邦东区</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2020-12-01 12:38:03</t>
+          <t>2020-12-01 15:09:12</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>65312719521212477X</t>
+          <t>231224199901079112</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>黎强</t>
+          <t>刘辉</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>15824171507</t>
+          <t>13588380680</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>119.932706608028</v>
+        <v>119.910831936552</v>
       </c>
       <c r="F64" t="n">
-        <v>30.050724801629</v>
+        <v>30.087445577424</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道金平路15号东方茂购物中心</t>
+          <t>浙江省杭州市富阳区银湖街道周长线</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2020-12-01 12:17:36</t>
+          <t>2020-12-01 15:16:18</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>130923199605033053</t>
+          <t>42092319931018251X</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>王秀英</t>
+          <t>毕彬</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>18768187282</t>
+          <t>13645815561</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>119.77364</v>
+        <v>119.960484596484</v>
       </c>
       <c r="F65" t="n">
-        <v>30.00227</v>
+        <v>30.051685506887</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇宝万线</t>
+          <t>浙江省杭州市富阳区富春街道龙浦街128号富阳龙浦大酒店</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2020-12-01 12:08:36</t>
+          <t>2020-12-01 15:25:31</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>630223201309169386</t>
+          <t>620724200208057999</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>林欣</t>
+          <t>鲁帅</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>15397123912</t>
+          <t>18658808055</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>119.94152</v>
+        <v>119.94854864858</v>
       </c>
       <c r="F66" t="n">
-        <v>30.06786</v>
+        <v>30.058028610008</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道新汇社区居务监督委员会北都荟公寓</t>
+          <t>浙江省杭州市富阳区富春街道孙权路28-2号现代技术培训学校</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2020-12-01 11:55:45</t>
+          <t>2020-12-01 15:36:09</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>140000197111029467</t>
+          <t>360826200002072688</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>萧海燕</t>
+          <t>严秀云</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>15925626674</t>
+          <t>13588397358</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>119.50874421565</v>
+        <v>119.792536773035</v>
       </c>
       <c r="F67" t="n">
-        <v>30.065402515467</v>
+        <v>29.884492806711</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>浙江省杭州市桐庐县分水镇兑百线</t>
+          <t>浙江省杭州市富阳区新桐乡桐洲绿道桐洲岛</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2020-12-01 11:52:26</t>
+          <t>2020-12-01 15:40:12</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>451402200207223734</t>
+          <t>440303199007136727</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>张斌</t>
+          <t>刘洋</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>13732236310</t>
+          <t>13588282970</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>119.93773524959</v>
+        <v>119.715405693318</v>
       </c>
       <c r="F68" t="n">
-        <v>30.05909982042</v>
+        <v>29.878966732299</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道文居街德邻公寓</t>
+          <t>浙江省杭州市富阳区渌渚镇大俞线</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2020-12-01 11:40:32</t>
+          <t>2020-12-01 15:48:22</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>640105200211029288</t>
+          <t>150122196009192963</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>张莹</t>
+          <t>李建军</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>15158845772</t>
+          <t>15858160116</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>119.966768963353</v>
+        <v>119.946324623285</v>
       </c>
       <c r="F69" t="n">
-        <v>30.133722600522</v>
+        <v>30.066249466767</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区银湖街道龙溪北路</t>
+          <t>浙江省杭州市富阳区富春街道公望街虎山雅苑</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2020-12-01 11:38:10</t>
+          <t>2020-12-01 16:10:20</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>441223198805172374</t>
+          <t>433124199012225830</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>余波</t>
+          <t>刘伟</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>13968052087</t>
+          <t>13605574551</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>119.950429002502</v>
+        <v>119.939331287876</v>
       </c>
       <c r="F70" t="n">
-        <v>30.051439174845</v>
+        <v>30.037166138909</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道渔种场路64号</t>
+          <t>浙江省杭州市富阳区富春街道文教路杭州富阳水务管道安装有限公司</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2020-12-01 11:35:34</t>
+          <t>2020-12-01 16:22:17</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>610627199601262610</t>
+          <t>513226199904235573</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>刘桂花</t>
+          <t>李欣</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>13429178089</t>
+          <t>13221828587</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>119.960879653585</v>
+        <v>119.936079476613</v>
       </c>
       <c r="F71" t="n">
-        <v>30.130014881814</v>
+        <v>30.062299368257</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区银湖街道上上线</t>
+          <t>浙江省杭州市富阳区富春街道郦城</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2020-12-01 11:32:02</t>
+          <t>2020-12-01 16:24:38</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>360827200012163053</t>
+          <t>610302199809281040</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>姜帆</t>
+          <t>赵丽丽</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13705711539</t>
+          <t>15824171348</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>119.937732806213</v>
+        <v>119.733700301888</v>
       </c>
       <c r="F72" t="n">
-        <v>30.052326877704</v>
+        <v>29.964790850403</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道凤凰小区</t>
+          <t>浙江省杭州市富阳区新登镇裕达饼家(新兴路店)</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2020-12-01 11:23:24</t>
+          <t>2020-12-01 16:27:43</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>361103201504145712</t>
+          <t>530481201904041070</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>向玉华</t>
+          <t>温强</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>13868163877</t>
+          <t>15867171758</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>119.94824</v>
+        <v>119.736853485196</v>
       </c>
       <c r="F73" t="n">
-        <v>30.06749</v>
+        <v>29.98939705182</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道天时苑(西区)天时苑西区</t>
+          <t>浙江省杭州市富阳区新登镇四号路</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2020-12-01 11:20:14</t>
+          <t>2020-12-01 16:29:09</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>370285199711144158</t>
+          <t>522627198302188970</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>李丹</t>
+          <t>杨云</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>13456836266</t>
+          <t>18329188508</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>119.975811008628</v>
+        <v>119.93543129835</v>
       </c>
       <c r="F74" t="n">
-        <v>30.02174502131</v>
+        <v>30.058400180538</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区春江街道春江街道直塘村文化活动中心</t>
+          <t>浙江省杭州市富阳区富春街道德邻公寓富阳区永兴学校</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2020-12-01 11:08:06</t>
+          <t>2020-12-01 16:31:49</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>350629198511195738</t>
+          <t>141029200007046791</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>张伟</t>
+          <t>吴金凤</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>13675875155</t>
+          <t>13968174817</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>119.94824</v>
+        <v>120.028376222184</v>
       </c>
       <c r="F75" t="n">
-        <v>30.06749</v>
+        <v>30.064818696745</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道天时苑(西区)天时苑西区</t>
+          <t>浙江省杭州市富阳区东洲街道湖上沙村</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2020-12-01 10:49:36</t>
+          <t>2020-12-01 16:31:54</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>632622196512049711</t>
+          <t>530722200207202520</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>张红</t>
+          <t>魏强</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>15067175728</t>
+          <t>13819164910</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>119.908879053854</v>
+        <v>119.920751734744</v>
       </c>
       <c r="F76" t="n">
-        <v>30.068399940499</v>
+        <v>30.063992918354</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道阳陂湖小火车南站阳陂湖P1停车场</t>
+          <t>浙江省杭州市富阳区富春街道西环北路225号</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2020-12-01 10:46:02</t>
+          <t>2020-12-01 16:45:08</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>320282199603151918</t>
+          <t>623025199904234990</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>钟辉</t>
+          <t>王宁</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>18258212106</t>
+          <t>15988879169</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>120.003246763257</v>
+        <v>119.746293071808</v>
       </c>
       <c r="F77" t="n">
-        <v>30.052777473716</v>
+        <v>30.000392682626</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区东洲街道何埭机埠</t>
+          <t>浙江省杭州市富阳区新登镇302省道</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2020-12-01 10:44:48</t>
+          <t>2020-12-01 16:58:25</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>532601201001289404</t>
+          <t>120102198805063327</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>叶玉英</t>
+          <t>李强</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>13588760817</t>
+          <t>15382328993</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>119.752260956386</v>
+        <v>119.8514063421</v>
       </c>
       <c r="F78" t="n">
-        <v>30.003557215076</v>
+        <v>29.988830761241</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇军堰路生威新能源</t>
+          <t>浙江省杭州市富阳区鹿山街道大树下</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2020-12-01 10:39:08</t>
+          <t>2020-12-01 17:03:16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>150825200311221952</t>
+          <t>331022199412259702</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>龚凯</t>
+          <t>邵晨</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>15088698899</t>
+          <t>18324490018</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>119.878397077327</v>
+        <v>119.93654794656</v>
       </c>
       <c r="F79" t="n">
-        <v>30.042040616969</v>
+        <v>30.054769047965</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道320国道辅路</t>
+          <t>浙江省杭州市富阳区富春街道飞虹·丁香花园(金桥北路)</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2020-12-01 10:35:20</t>
+          <t>2020-12-01 17:07:01</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>411500199808167299</t>
+          <t>441802199205254646</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>陈帅</t>
+          <t>杨兵</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>18067904810</t>
+          <t>15967114462</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>119.92601</v>
+        <v>119.978243327095</v>
       </c>
       <c r="F80" t="n">
-        <v>29.9352</v>
+        <v>30.077620959272</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区环山乡G25长深高速</t>
+          <t>浙江省杭州市富阳区东洲街道杭州爱派克船舶有限公司佑昌意菲司图(杭州)金属制品有限公司</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2020-12-01 10:31:53</t>
+          <t>2020-12-01 17:12:08</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>341102199204084962</t>
+          <t>371721200011076141</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>李秀芳</t>
+          <t>齐宁</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>13706505205</t>
+          <t>13588390997</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>119.88067</v>
+        <v>119.866428407807</v>
       </c>
       <c r="F81" t="n">
-        <v>30.12405</v>
+        <v>30.039808618221</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区银湖街道杭州市富阳区银湖街道新义小学</t>
+          <t>浙江省杭州市富阳区富春街道唯益生态农场</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2020-12-01 10:26:43</t>
+          <t>2020-12-01 17:12:40</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>653123198508197589</t>
+          <t>520325199808286280</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>王芳</t>
+          <t>张宁</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>15888825716</t>
+          <t>15088651898</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>119.950580984148</v>
+        <v>119.66851</v>
       </c>
       <c r="F82" t="n">
-        <v>30.052734196765</v>
+        <v>29.98639</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道新兴路122号百合景苑</t>
+          <t>浙江省杭州市富阳区胥口镇泥塍头</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2020-12-01 10:26:05</t>
+          <t>2020-12-01 17:14:27</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>350800199602085481</t>
+          <t>21110420160301771X</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>刘淑兰</t>
+          <t>朱平</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>13868127754</t>
+          <t>18058819611</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>119.872802703836</v>
+        <v>119.609769267959</v>
       </c>
       <c r="F83" t="n">
-        <v>29.988073551047</v>
+        <v>30.034007878132</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区鹿山街道杭州安澜海业动力机械有限公司</t>
+          <t>浙江省杭州市富阳区洞桥镇胥高线</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2020-12-01 10:23:40</t>
+          <t>2020-12-01 17:17:21</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>230123199105253957</t>
+          <t>140404201803243997</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>王萍</t>
+          <t>刘雪</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>15568233366</t>
+          <t>13911869797</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>119.941568251921</v>
+        <v>119.912227902269</v>
       </c>
       <c r="F84" t="n">
-        <v>30.072021320619</v>
+        <v>30.009356612782</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道富春印象金座富春新天地</t>
+          <t>浙江省杭州市富阳区鹿山街道富冶</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2020-12-01 10:20:20</t>
+          <t>2020-12-01 17:21:38</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>610803201510213143</t>
+          <t>320118201302072910</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>张坤</t>
+          <t>曾旭</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>13968071566</t>
+          <t>13626713248</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>119.940044577139</v>
+        <v>119.914827000385</v>
       </c>
       <c r="F85" t="n">
-        <v>30.053073402269</v>
+        <v>30.054731999654</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道凤浦路</t>
+          <t>浙江省杭州市富阳区富春街道金秋大道57号</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2020-12-01 10:20:09</t>
+          <t>2020-12-01 17:21:56</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>230183199606275181</t>
+          <t>130321198603056999</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>李淑兰</t>
+          <t>杨志强</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>13584838199</t>
-        </is>
-      </c>
-      <c r="E86" t="n">
-        <v>119.971528287016</v>
-      </c>
-      <c r="F86" t="n">
-        <v>30.038272696524</v>
+          <t>13968019333</t>
+        </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区春江街道大桥南路</t>
+          <t>error: 输入坐标不全!</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2020-12-01 09:08:36</t>
+          <t>2020-12-01 17:29:05</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>632723198403048091</t>
+          <t>371425199411046877</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>吴岩</t>
+          <t>胡婷</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>15824190404</t>
+          <t>17706442283</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>119.736699662198</v>
+        <v>119.92575</v>
       </c>
       <c r="F87" t="n">
-        <v>29.96761302358</v>
+        <v>30.02332</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇登城北路19号</t>
+          <t>浙江省杭州市富阳区鹿山街道驯雉小学</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2020-12-01 09:04:14</t>
+          <t>2020-12-01 17:38:40</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>430423198406157378</t>
+          <t>520281201703269746</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>汪秀梅</t>
+          <t>孙建平</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>13221099822</t>
+          <t>13968164976</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>119.87082</v>
+        <v>119.937601140995</v>
       </c>
       <c r="F88" t="n">
-        <v>29.97833</v>
+        <v>30.030894926297</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区鹿山街道S43杭州绕城西复线</t>
+          <t>浙江省杭州市富阳区富春街道富春第七小学</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2020-12-01 08:54:56</t>
+          <t>2020-12-01 17:40:18</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>440114200005255494</t>
+          <t>431302199901045021</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>冉晨</t>
+          <t>罗岩</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>15658115330</t>
+          <t>15957128398</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>119.925901060393</v>
+        <v>119.910291130682</v>
       </c>
       <c r="F89" t="n">
-        <v>30.070107726686</v>
+        <v>30.063990017737</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道金苑路</t>
+          <t>浙江省杭州市富阳区富春街道公望街1165号汉邦钢材市场北区</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2020-12-01 08:53:05</t>
+          <t>2020-12-01 17:50:33</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>450108200402126076</t>
+          <t>130582199505259141</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>王鹏</t>
+          <t>孙瑞</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>13567138273</t>
+          <t>13336027313</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>119.946904588043</v>
+        <v>119.93635505368</v>
       </c>
       <c r="F90" t="n">
-        <v>30.068024227572</v>
+        <v>30.053672876579</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道天时苑(西区)金门东望大厦</t>
+          <t>浙江省杭州市富阳区富春街道凤浦社区飞虹·丁香花园(金桥北路)</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2020-12-01 08:42:08</t>
+          <t>2020-12-01 18:06:50</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>331121200011172184</t>
+          <t>410721198907254459</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>范淑英</t>
+          <t>胡琴</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>15858189066</t>
+          <t>13588396058</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>119.940073401748</v>
+        <v>119.744834</v>
       </c>
       <c r="F91" t="n">
-        <v>30.049084693107</v>
+        <v>30.005376</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道金都铭苑(秋月路)金都铭苑东区</t>
+          <t>浙江省杭州市富阳区新登镇沃新线</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2020-12-01 08:24:41</t>
+          <t>2020-12-01 18:08:38</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>370613199408051995</t>
+          <t>140703201909156648</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>郭勇</t>
+          <t>江桂荣</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>13588818578</t>
+          <t>13675876638</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>119.95848734533</v>
+        <v>119.962443727165</v>
       </c>
       <c r="F92" t="n">
-        <v>30.055637341849</v>
+        <v>30.05409731211</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道大桥路63号明裕花苑(大桥路)</t>
+          <t>浙江省杭州市富阳区富春街道大桥路159号富阳区城市森林公园</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2020-12-01 08:24:36</t>
+          <t>2020-12-01 18:15:39</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>310104199001029361</t>
+          <t>420702198710241956</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>周佳</t>
+          <t>陈秀荣</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>18758087628</t>
+          <t>18327553759</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>119.748167457896</v>
+        <v>119.891836841929</v>
       </c>
       <c r="F93" t="n">
-        <v>30.001813667236</v>
+        <v>30.05821063413</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区新登镇贝山路浙江新源服装有限公司</t>
+          <t>浙江省杭州市富阳区富春街道双峰山</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2020-12-01 08:20:56</t>
+          <t>2020-12-01 18:18:00</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>610304200312125147</t>
+          <t>320612200909197407</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>卢玉兰</t>
+          <t>王杰</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>13803990917</t>
-        </is>
+          <t>18314899806</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>120.030650057354</v>
+      </c>
+      <c r="F94" t="n">
+        <v>30.033001385081</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>error: 输入坐标不全!</t>
+          <t>浙江省杭州市富阳区灵桥镇春胜线</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2020-12-01 08:18:05</t>
+          <t>2020-12-01 18:22:06</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>659006201203234308</t>
+          <t>130530199303287789</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>赵云</t>
+          <t>纪欣</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>18658042800</t>
+          <t>15972406141</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>119.959673357473</v>
+        <v>119.988072555233</v>
       </c>
       <c r="F95" t="n">
-        <v>30.053757333239</v>
+        <v>30.069137945355</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道达夫路145号</t>
+          <t>浙江省杭州市富阳区东洲街道高尔夫路537号富阳东洲民丰小学</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2020-12-01 08:18:00</t>
+          <t>2020-12-01 18:29:16</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>530125198308111288</t>
+          <t>620502200404014890</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>杨丽</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>15888809563</t>
+          <t>张彬</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>119.974322358456</v>
+        <v>119.697746222762</v>
       </c>
       <c r="F96" t="n">
-        <v>30.162255520543</v>
+        <v>29.984817036958</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区银湖街道九龙仓·雍景山九龙仓·雍景山城</t>
+          <t>浙江省杭州市富阳区胥口镇05省道</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2020-12-01 08:12:47</t>
+          <t>2020-12-01 18:29:40</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>230605198211158179</t>
+          <t>430602199608232632</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>李平</t>
+          <t>裴璐</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>13588372438</t>
+          <t>13362568609</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>119.985952799662</v>
+        <v>119.893050007208</v>
       </c>
       <c r="F97" t="n">
-        <v>30.067752766367</v>
+        <v>30.064440002077</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区东洲街道浙江富春江光电科技有限公司富春江集团光通信工业园</t>
+          <t>浙江省杭州市富阳区富春街道杭州潮汛流体控制科技有限公司</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2020-12-01 08:08:42</t>
+          <t>2020-12-01 18:31:10</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>440800196508026141</t>
+          <t>21072619701115157X</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>黄霞</t>
+          <t>王兵</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>13357111728</t>
+          <t>15158830484</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>119.946324623285</v>
+        <v>119.954771379323</v>
       </c>
       <c r="F98" t="n">
-        <v>30.066249466767</v>
+        <v>30.057509470828</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道公望街虎山雅苑</t>
+          <t>浙江省杭州市富阳区富春街道光明路9-1号</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2020-12-01 08:07:16</t>
+          <t>2020-12-01 18:31:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>321300199611276069</t>
+          <t>511324199305085738</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>周玉梅</t>
+          <t>杨利</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>18758002725</t>
+          <t>13777853631</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>119.935197936995</v>
+        <v>119.87356</v>
       </c>
       <c r="F99" t="n">
-        <v>30.053488762548</v>
+        <v>29.99376</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道永兴花园凤凰苑(凤浦路)</t>
+          <t>浙江省杭州市富阳区鹿山街道永盛科技有限公司(流体事业部)</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2020-12-01 08:04:40</t>
+          <t>2020-12-01 18:31:49</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>211282199509102728</t>
+          <t>360900200004277902</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>敖英</t>
+          <t>赵旭</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>13777491569</t>
+          <t>15967192402</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>119.873099285498</v>
+        <v>119.938346115923</v>
       </c>
       <c r="F100" t="n">
-        <v>29.988102645403</v>
+        <v>30.05770211121</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区鹿山街道杭州安澜海业动力机械有限公司</t>
+          <t>浙江省杭州市富阳区富春街道文教北路永兴学校教师公寓</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2020-12-01 08:04:35</t>
+          <t>2020-12-01 18:31:49</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>140403201804261912</t>
+          <t>220881199511247851</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>郑莹</t>
+          <t>张凤英</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>13362144407</t>
+          <t>15669536808</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>119.920835130529</v>
+        <v>119.971807169923</v>
       </c>
       <c r="F101" t="n">
-        <v>30.013759836072</v>
+        <v>30.031203474998</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区鹿山街道福济庙</t>
+          <t>浙江省杭州市富阳区春江街道上海外国语大学附属杭州学校(建设中)</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2020-12-01 08:00:31</t>
+          <t>2020-12-01 18:36:23</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>421222199809034969</t>
+          <t>45092419970517118X</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>陈琴</t>
+          <t>张阳</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>13858071281</t>
+          <t>13777359971</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>119.906691219552</v>
+        <v>119.961144852051</v>
       </c>
       <c r="F102" t="n">
-        <v>30.048983698148</v>
+        <v>30.030052570865</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道华虹路辰春澜城(建设中)</t>
+          <t>浙江省杭州市富阳区春江街道江南中学</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2020-12-01 07:56:16</t>
+          <t>2020-12-01 19:03:05</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>130481199512241239</t>
+          <t>130302198306122348</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>赵琳</t>
+          <t>江龙</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>13967103871</t>
+          <t>13706816295</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>119.936719993773</v>
+        <v>119.988101918469</v>
       </c>
       <c r="F103" t="n">
-        <v>30.043488856435</v>
+        <v>30.069178386718</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道城市花园(秦望路)龙祥城市花园</t>
+          <t>浙江省杭州市富阳区东洲街道高尔夫路537号富阳东洲民丰小学</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2020-12-01 07:55:28</t>
+          <t>2020-12-01 19:16:35</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>450324199806012791</t>
+          <t>511526199609013761</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>余静</t>
+          <t>高倩</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>18858121141</t>
+          <t>15988180938</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>119.884279760809</v>
+        <v>119.917848478986</v>
       </c>
       <c r="F104" t="n">
-        <v>30.117161307504</v>
+        <v>30.066553789586</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区银湖街道423县道</t>
+          <t>浙江省杭州市富阳区富春街道孙油线</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2020-12-01 07:49:19</t>
+          <t>2020-12-01 19:20:55</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>51118119951001381X</t>
+          <t>421223199805018239</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>吴鹏</t>
+          <t>吴勇</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>15869103863</t>
-        </is>
-      </c>
-      <c r="E105" t="n">
-        <v>119.839629365219</v>
-      </c>
-      <c r="F105" t="n">
-        <v>29.985965842432</v>
+          <t>18958171357</t>
+        </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区鹿山街道华家</t>
+          <t>error: 输入坐标不全!</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2020-12-01 07:40:36</t>
+          <t>2020-12-01 19:21:19</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>420000196511075182</t>
+          <t>130626199411096219</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>方玉华</t>
+          <t>蒲柳</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>13858048604</t>
+          <t>15324476439</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>120.09642</v>
+        <v>119.72229</v>
       </c>
       <c r="F106" t="n">
-        <v>30.04937</v>
+        <v>29.9667</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区渔山乡渔葛线</t>
+          <t>浙江省杭州市富阳区新登镇430县道</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2020-12-01 07:22:28</t>
+          <t>2020-12-01 19:27:51</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>330402200511053516</t>
+          <t>140727199902258044</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>李玉</t>
+          <t>裘亮</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>15267012370</t>
+          <t>15258868990</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>119.934402483888</v>
+        <v>119.95238</v>
       </c>
       <c r="F107" t="n">
-        <v>30.090534554371</v>
+        <v>30.07537</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区银湖街道万达同心湾(建设中)杭州富阳万达广场</t>
+          <t>浙江省杭州市富阳区富春街道庭庐餐厅融创富春壹号院</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2020-12-01 07:18:18</t>
+          <t>2020-12-01 19:58:38</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>511903201305174205</t>
+          <t>310151201609227483</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>张玉珍</t>
+          <t>黄彬</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>15068120595</t>
+          <t>18768118774</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>119.920252972396</v>
+        <v>119.870459933587</v>
       </c>
       <c r="F108" t="n">
-        <v>30.050301859895</v>
+        <v>29.914567752373</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道浪漫香槟(东区)浪漫香槟东区</t>
+          <t>浙江省杭州市富阳区场口镇瓜桥江绿道</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2020-12-01 07:12:02</t>
+          <t>2020-12-01 20:12:34</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>469029200310029400</t>
+          <t>410800198209196611</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>程杰</t>
+          <t>张辉</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>13806516227</t>
+          <t>18357147883</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>119.730270000247</v>
+        <v>119.971528287016</v>
       </c>
       <c r="F109" t="n">
-        <v>29.936659999961</v>
+        <v>30.038272696524</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区渌渚镇碧沼寺</t>
+          <t>浙江省杭州市富阳区春江街道大桥南路</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2020-12-01 07:11:06</t>
+          <t>2020-12-01 20:46:16</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>410425198608116258</t>
+          <t>361127200007015606</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>胡超</t>
+          <t>王丽</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>13606609521</t>
+          <t>15938399252</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>119.628240003265</v>
+        <v>119.946664272439</v>
       </c>
       <c r="F110" t="n">
-        <v>29.961270004524</v>
+        <v>30.046655271192</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区胥口镇水坞水库</t>
+          <t>浙江省杭州市富阳区富春街道回春路回春路-道路停车位</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2020-12-01 06:33:26</t>
+          <t>2020-12-01 21:13:39</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>331024199501036087</t>
+          <t>230805198304179586</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>阎春梅</t>
+          <t>李桂兰</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>15156483403</t>
+          <t>15085699499</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>119.885075462635</v>
+        <v>119.75001</v>
       </c>
       <c r="F111" t="n">
-        <v>29.897829252702</v>
+        <v>29.99805</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区常安镇双隆控股集团</t>
+          <t>浙江省杭州市富阳区新登镇5号路</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2020-12-01 06:29:55</t>
+          <t>2020-12-01 21:20:13</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>130110201406057962</t>
+          <t>320831199506081068</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>王娟</t>
+          <t>吴帅</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>13738014816</t>
-        </is>
+          <t>15057188534</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>119.934256663262</v>
+      </c>
+      <c r="F112" t="n">
+        <v>30.038822422433</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>error: 输入坐标不全!</t>
+          <t>浙江省杭州市富阳区富春街道南渠绿道</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2020-12-01 05:58:00</t>
+          <t>2020-12-01 21:21:10</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>610524199407192917</t>
+          <t>211381199612278296</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>蔡秀云</t>
+          <t>林红霞</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>18281858028</t>
-        </is>
+          <t>13500599252</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>119.945421709799</v>
+      </c>
+      <c r="F113" t="n">
+        <v>30.045358805853</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>error: 输入坐标不全!</t>
+          <t>浙江省杭州市富阳区富春街道菜市街70号</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2020-12-01 05:43:52</t>
+          <t>2020-12-01 22:21:17</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>440200198007168914</t>
+          <t>422825198810114454</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>冯宇</t>
+          <t>张荣</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>15157132991</t>
+          <t>18248480965</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>119.934881684961</v>
+        <v>119.944296584982</v>
       </c>
       <c r="F114" t="n">
-        <v>30.063084431323</v>
+        <v>30.097262635875</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>浙江省杭州市富阳区富春街道文采路202号金色家园(金桥北路)</t>
+          <t>浙江省杭州市富阳区银湖街道高富路富通高桥工场</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>